<commit_message>
Add: new motivational quotes
</commit_message>
<xml_diff>
--- a/El Professor/data/motivationquotes.xlsx
+++ b/El Professor/data/motivationquotes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Patrick/Documents/STUDIUM DBM_18/01 Classes/3. Semester/PROG2/prog2/El Professor/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B772A01-3E33-DC45-8701-C3C6F983E362}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76215AB8-7A9E-FF45-BF48-7D3E742C33FC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="15260" yWindow="460" windowWidth="13540" windowHeight="17540" xr2:uid="{45AF6C6F-2A92-6242-81BF-74C356645E94}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Who cares if I'm pretty if I fail my finals? - Rory Gilmore</t>
   </si>
@@ -81,6 +81,9 @@
   </si>
   <si>
     <t>I'm not great at the advice. Can I interest you in a sarcastic comment? - Chandler Bing</t>
+  </si>
+  <si>
+    <t>42 - Deep Thought</t>
   </si>
 </sst>
 </file>
@@ -116,8 +119,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -432,10 +438,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03B60DD5-9443-BD4A-9414-9D31B4A8E3ED}">
-  <dimension ref="A1:A16"/>
+  <dimension ref="A1:A17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -524,6 +530,11 @@
         <v>15</v>
       </c>
     </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>